<commit_message>
Working on resubmission pieces.
</commit_message>
<xml_diff>
--- a/Submissions/8-TheEnergyJournal-Resubmission/Other files/Responses to MPC reviewers November 2024.xlsx
+++ b/Submissions/8-TheEnergyJournal-Resubmission/Other files/Responses to MPC reviewers November 2024.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundPaper2022/Submissions/8-TheEnergyJournal-Resubmission/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundPaper2022/Submissions/8-TheEnergyJournal-Resubmission/Other files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E4D108-7318-B545-A30C-D29CA73C9E6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64984261-020F-F342-BFAC-D3C7D51DFE40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -265,11 +265,6 @@
 This point has reinforced the importance of highlighting our objectives. In response, we which you added a new footnote in Section 1.4 of Part I: "This objective may mean that some aspects of the development of the framework will seem obvious to energy analysts while other aspects will seem obvious to economists."</t>
   </si>
   <si>
-    <t>Thank you for your comment and pointing out the very large increase in lamp running time. We actually use an elasticity on the lower end of Borenstein's (2015) elasticity range of 0.4 to 0.8. Effectively our results indicate that a lamp is being used 7 instead of 3 hours a day. This may mean that a lamp isn't turned off when device users leave a room or the house for short times - something that the authors find anecdotal evidence for in their daily lives. However, we agree that it is important to distinguish this rebound effect from one where the additional or more powerful lamps would be added. Here, the size of the rebound would be affected in two ways: first, since more cash would be spent on a second lamp or presumably also on a more powerful single lamp, the income effect which includes the (negative) savings from emplacement as you perspicuously pointed out, would become smaller. At the same time, substitution effect rebound would become larger.
-To address these points, we added a footnote in Section 3.2.1 Numerical results: Lamp example.
-Thank you for this helpful comment.</t>
-  </si>
-  <si>
     <t>Thank you for this insightful comment. We agree with the reviewer that in the aggregate, technology adoption usually follows a logistic (or s) curve. However, our framework is focused on individual machines. So the original sentence and the S-curve adoption are not really applicable. 
 To address this comment, we deleted the text justifying our approach, namely "A justification for spreading embodied energy and purchase costs comes from considering device replacements by many consumers across several years. In the aggregate, evenly spaced (in time) replacements work out to the same embodied energy in every period." We already say our approach is a simplification ("For simplicity, we spread all embodied energy over the lifetime of the device for a constant embodied energy rate ($\rate{E}_{emb}$)%.")
 Then, we modified the sentence in question to the following: "For simplicity, we spread all embodied energy evenly over the lifetime of the device which gives a constant embodied energy rate ($\rate{E}_{emb}$)."
@@ -351,6 +346,13 @@
       </rPr>
       <t>Any (positive or negative) adjustment in income due to emplacement (measured as net income, N_dot_star) is added to the freed cash (G_dot) spent in the income effect.</t>
     </r>
+  </si>
+  <si>
+    <t>Thank you for your comment and pointing out the very large increase in lamp running time. We actually use an elasticity on the least-negative end of Borenstein's (2015) elasticity range of -0.4 to -0.8 (as discussed in Table 6. Effectively, our results indicate that a lamp is being used 7 instead of 3 hours per day. This may mean that a lamp isn't turned off when device users leave a room or the house for short times - something that we find anecdotal evidence for in our daily lives. However, we agree that it is important to distinguish this rebound effect from one where the additional or more powerful lamps would be added. 
+To that end, we now call out the Schleich (2014) reference, because it estiates "burn time" rebound. However, Schleich's methodology relies upon respondent self-reporting of additional burn time for lamps. In-home measurements would have been better. Regardless, an elasticity value can be back-calculated from their burn time rebound value: -0.13.
+We also note that Fouquet (2011) finds economy-wide elasticity to be -0.6. The single-device rebound elasticity is expected to be less negative, another reason why we choose -0.4 for our preferred value.
+We pull all of this together in a new section 4.4 investigating the sensitivity of total rebound on the uncompensated own price elasticity of energy service consumption. In that section, we use the three elasticity values to calculate total rebound and find total rebound for the lamp example is 55% with elasticity = -0.13, 67% with elasticity = -0.4 (our preferred value), and 81.7% with elasticity = -0.6. We also pull the elasticity sensitivity graph for the lamp forward from the appendix to illustrate the sensitivities involved for each component of rebound.
+Thank you again for this helpful comment.</t>
   </si>
 </sst>
 </file>
@@ -683,16 +685,16 @@
   <dimension ref="A1:E760"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="6.33203125" customWidth="1"/>
     <col min="2" max="2" width="10.1640625" customWidth="1"/>
-    <col min="3" max="3" width="62.5" customWidth="1"/>
-    <col min="4" max="4" width="84.6640625" customWidth="1"/>
+    <col min="3" max="3" width="39" customWidth="1"/>
+    <col min="4" max="4" width="46" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
     <col min="6" max="6" width="26.33203125" customWidth="1"/>
   </cols>
@@ -937,7 +939,7 @@
         <v>40</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E17" s="4"/>
     </row>
@@ -1034,7 +1036,7 @@
         <v>35</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E24" s="4"/>
     </row>
@@ -1053,7 +1055,7 @@
       </c>
       <c r="E25" s="4"/>
     </row>
-    <row r="26" spans="1:5" ht="196" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" ht="332" x14ac:dyDescent="0.15">
       <c r="A26" s="1">
         <v>2</v>
       </c>
@@ -1064,7 +1066,7 @@
         <v>38</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E26" s="4"/>
     </row>

</xml_diff>